<commit_message>
search for a second key in yahoo source if 'currentPrice' is not found
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -2,81 +2,281 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="8016" windowWidth="14808" xWindow="240" yWindow="108"/>
+    <workbookView xWindow="0" yWindow="96" windowWidth="19416" windowHeight="11016"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+  <si>
+    <t>ba</t>
+  </si>
   <si>
     <t>epd</t>
   </si>
   <si>
-    <t>otcm</t>
+    <t>msft</t>
+  </si>
+  <si>
+    <t>amzn</t>
+  </si>
+  <si>
+    <t>ge</t>
+  </si>
+  <si>
+    <t>xom</t>
+  </si>
+  <si>
+    <t>cvx</t>
+  </si>
+  <si>
+    <t>apc</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>met</t>
+  </si>
+  <si>
+    <t>cnp</t>
+  </si>
+  <si>
+    <t>pfe</t>
+  </si>
+  <si>
+    <t>sfm</t>
+  </si>
+  <si>
+    <t>bac</t>
+  </si>
+  <si>
+    <t>bhf</t>
+  </si>
+  <si>
+    <t>rig</t>
+  </si>
+  <si>
+    <t>feye</t>
+  </si>
+  <si>
+    <t>al</t>
+  </si>
+  <si>
+    <t>gild</t>
+  </si>
+  <si>
+    <t>hd</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>csco</t>
+  </si>
+  <si>
+    <t>alb</t>
+  </si>
+  <si>
+    <t>ewj</t>
+  </si>
+  <si>
+    <t>jpxn</t>
+  </si>
+  <si>
+    <t>xlv</t>
+  </si>
+  <si>
+    <t>kre</t>
+  </si>
+  <si>
+    <t>xlre</t>
+  </si>
+  <si>
+    <t>dwdp</t>
+  </si>
+  <si>
+    <t>vgsnx</t>
+  </si>
+  <si>
+    <t>gccsx</t>
+  </si>
+  <si>
+    <t>nvda</t>
+  </si>
+  <si>
+    <t>smapx</t>
+  </si>
+  <si>
+    <t>vpmax</t>
+  </si>
+  <si>
+    <t>vscpx</t>
+  </si>
+  <si>
+    <t>glfox</t>
+  </si>
+  <si>
+    <t>baba</t>
+  </si>
+  <si>
+    <t>uri</t>
+  </si>
+  <si>
+    <t>avgo</t>
   </si>
   <si>
     <t>lvmuy</t>
   </si>
   <si>
-    <t>aapl</t>
-  </si>
-  <si>
-    <t>msft</t>
-  </si>
-  <si>
-    <t>ba</t>
-  </si>
-  <si>
-    <t>ip</t>
-  </si>
-  <si>
-    <t>vgsnx</t>
-  </si>
-  <si>
-    <t>65.52</t>
-  </si>
-  <si>
-    <t>28.85</t>
-  </si>
-  <si>
-    <t>28.35</t>
-  </si>
-  <si>
-    <t>221.3</t>
-  </si>
-  <si>
-    <t>108.21</t>
-  </si>
-  <si>
-    <t>349.28</t>
-  </si>
-  <si>
-    <t>51.71</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> id="atomic" class="NoJs featurephone" lang="en-US"&gt;&lt;head prefix="og: http://ogp.me/ns#"&gt;&lt;script&gt;window.performance &amp;&amp; window.performance.mark &amp;&amp; window.performance.mark('PageStart');&lt;/script&gt;&lt;meta charset="utf-8"/&gt;&lt;title&gt;VGSNX : Summary for Vanguard Real Estate Index Fund - Yahoo Finance&lt;/title&gt;&lt;meta name="keywords" content="VGSNX</t>
-  </si>
-  <si>
-    <t>18.18</t>
+    <t>82.92</t>
+  </si>
+  <si>
+    <t>12.68</t>
+  </si>
+  <si>
+    <t>359.8</t>
+  </si>
+  <si>
+    <t>117.38</t>
+  </si>
+  <si>
+    <t>63.01</t>
+  </si>
+  <si>
+    <t>68.58</t>
+  </si>
+  <si>
+    <t>29.23</t>
+  </si>
+  <si>
+    <t>9.45</t>
+  </si>
+  <si>
+    <t>46.53</t>
+  </si>
+  <si>
+    <t>28.92</t>
+  </si>
+  <si>
+    <t>42.96</t>
+  </si>
+  <si>
+    <t>28.22</t>
+  </si>
+  <si>
+    <t>30.37</t>
+  </si>
+  <si>
+    <t>41.97</t>
+  </si>
+  <si>
+    <t>11.75</t>
+  </si>
+  <si>
+    <t>16.68</t>
+  </si>
+  <si>
+    <t>45.68</t>
+  </si>
+  <si>
+    <t>73.38</t>
+  </si>
+  <si>
+    <t>113.37</t>
+  </si>
+  <si>
+    <t>209.07</t>
+  </si>
+  <si>
+    <t>113.89</t>
+  </si>
+  <si>
+    <t>1970.19</t>
+  </si>
+  <si>
+    <t>47.4</t>
+  </si>
+  <si>
+    <t>100.9</t>
+  </si>
+  <si>
+    <t>276.43</t>
+  </si>
+  <si>
+    <t>168.95</t>
+  </si>
+  <si>
+    <t>164.74</t>
+  </si>
+  <si>
+    <t>68.085</t>
+  </si>
+  <si>
+    <t>236.34</t>
+  </si>
+  <si>
+    <t>58.12</t>
+  </si>
+  <si>
+    <t>62.73</t>
+  </si>
+  <si>
+    <t>15.5</t>
+  </si>
+  <si>
+    <t>7.88</t>
+  </si>
+  <si>
+    <t>93.5</t>
+  </si>
+  <si>
+    <t>62.02</t>
+  </si>
+  <si>
+    <t>33.58</t>
+  </si>
+  <si>
+    <t>52.69</t>
+  </si>
+  <si>
+    <t>18.23</t>
+  </si>
+  <si>
+    <t>151.98</t>
+  </si>
+  <si>
+    <t>228.57</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -101,16 +301,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -124,10 +330,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -285,7 +491,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -294,13 +500,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -310,7 +516,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -319,7 +525,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -328,7 +534,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -338,12 +544,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -374,7 +580,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -393,7 +599,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -405,104 +611,361 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>